<commit_message>
Datos de excel modificados e imagenes nuevas subidas
</commit_message>
<xml_diff>
--- a/Datos_Investigacion.xlsx
+++ b/Datos_Investigacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelaleman/Desktop/face_recognition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF46C6EE-7806-9C47-8617-FA42C4A900D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA22CC9-A431-4B2D-960E-815D5EAB150C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="500" windowWidth="28040" windowHeight="14500" xr2:uid="{2385BAF8-FA20-D944-A807-663308FAC982}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2385BAF8-FA20-D944-A807-663308FAC982}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="177">
   <si>
     <t>nControl</t>
   </si>
@@ -71,18 +69,30 @@
     <t>Diego Alejandro De La Rocha Linarez</t>
   </si>
   <si>
+    <t>Manjarrez Rodelo Omar</t>
+  </si>
+  <si>
     <t>Brayan Mendoza Garcia</t>
   </si>
   <si>
     <t>Luis Xavier Acosta Chang</t>
   </si>
   <si>
+    <t>Roberto Carlos Saucedo Rodríguez</t>
+  </si>
+  <si>
     <t>Carlos Eduardo Padilla Pimentel</t>
   </si>
   <si>
+    <t>Alexis Guillén Ruiz</t>
+  </si>
+  <si>
     <t>Astrid Monserrat Echegarray Aceves</t>
   </si>
   <si>
+    <t>Portillo López Emma Daniela</t>
+  </si>
+  <si>
     <t>Luis Enrique Ojeda Lopez</t>
   </si>
   <si>
@@ -182,12 +192,18 @@
     <t>Sistemas Computacionales</t>
   </si>
   <si>
+    <t>Jatniel Alejandro Peña Vizcarra</t>
+  </si>
+  <si>
     <t>l21170432@culiacan.tecnm.mx</t>
   </si>
   <si>
     <t>Cesar Enrique Vazquez Cardenas</t>
   </si>
   <si>
+    <t>Angel Cardenas Quiñonez</t>
+  </si>
+  <si>
     <t>Cinthia Guadalupe Pinedo Garcia</t>
   </si>
   <si>
@@ -209,6 +225,9 @@
     <t>Sebastian Verdugo Bermudez</t>
   </si>
   <si>
+    <t>Sergio Jesus García Sanchez</t>
+  </si>
+  <si>
     <t>Ciencias Basicas</t>
   </si>
   <si>
@@ -248,55 +267,314 @@
     <t>l21170252@culiacan.tecnm.mx</t>
   </si>
   <si>
-    <t>Emma Daniela Portillo Lopez</t>
-  </si>
-  <si>
-    <t>Omar Manjarrez Rodelo</t>
-  </si>
-  <si>
-    <t>Angel Cardenas Quinonez</t>
-  </si>
-  <si>
-    <t>Alexis Guillen Ruiz</t>
-  </si>
-  <si>
-    <t>Sergio Jesus Garcia Sanchez</t>
-  </si>
-  <si>
-    <t>Roberto Carlos Saucedo Rodriguez</t>
-  </si>
-  <si>
-    <t>Jatniel Alejandro Pena Vizcarra</t>
-  </si>
-  <si>
-    <t>Alma Victoria Cuen Armenta</t>
-  </si>
-  <si>
-    <t>Brayan Alexis Amarillas Aviles</t>
-  </si>
-  <si>
-    <t>l21170298@culiacan.tecnm.mx</t>
-  </si>
-  <si>
-    <t>l21170236@culiacan.tecnm.mx</t>
+    <t>Javier Uribe Armenta</t>
+  </si>
+  <si>
+    <t>l21170497@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Jesus Omar Dominguez Lopez</t>
+  </si>
+  <si>
+    <t>l23170214@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Yael Aram Lugo Ojeda</t>
+  </si>
+  <si>
+    <t>l23170137@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>l23170115@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Juan Diego Carrillo Heredia</t>
+  </si>
+  <si>
+    <t>C17170977</t>
+  </si>
+  <si>
+    <t>Gabriel Roberto Pastor Varela</t>
+  </si>
+  <si>
+    <t>Industrial</t>
+  </si>
+  <si>
+    <t>Juan Carlos Terraza</t>
+  </si>
+  <si>
+    <t>l24170747@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Paul Eduardo Coronel Carrillo</t>
+  </si>
+  <si>
+    <t>l21170550@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Luis Antonio Peñuelas Lopez</t>
+  </si>
+  <si>
+    <t>l21170433@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Jesus Daniel Picos Gomzalez</t>
+  </si>
+  <si>
+    <t>l23170279@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Adrian Chavez Espinoza</t>
+  </si>
+  <si>
+    <t>l24270519@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Julio Esteban Beltran Cardenas</t>
+  </si>
+  <si>
+    <t>l24170488@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Erick David Rodriguez Meza</t>
+  </si>
+  <si>
+    <t>l24170713@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Alan Elihu Yanes Ayala</t>
+  </si>
+  <si>
+    <t>l23170907@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Daniel Eduardo Valdez Espinoza</t>
+  </si>
+  <si>
+    <t>l24170758@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Kevin Edgar Mexia Leon</t>
+  </si>
+  <si>
+    <t>l22170723@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Habram Alexander Cervantes Ojeda</t>
+  </si>
+  <si>
+    <t>l24171226@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Jose Yair Muñoz Ochoa</t>
+  </si>
+  <si>
+    <t>l21170694@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Luis Alan Trapero Martinez</t>
+  </si>
+  <si>
+    <t>l21171174@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Leonel Esteban Garcia Figueroa</t>
+  </si>
+  <si>
+    <t>l23170044@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Tics</t>
+  </si>
+  <si>
+    <t>Eduar Yair Aguirre Ceballos</t>
+  </si>
+  <si>
+    <t>l23170037@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Edlin Jaqueline Cruz Camargo</t>
+  </si>
+  <si>
+    <t>l23170042@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Jesus Alejandro Quintero Castro</t>
+  </si>
+  <si>
+    <t>l23170054@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Vanessa Guadalupe Hernandez Ramos</t>
+  </si>
+  <si>
+    <t>l23170050@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Misael Ruiz Elizalde</t>
+  </si>
+  <si>
+    <t>l23170055@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Meza Escobar Cesar Eduardo</t>
+  </si>
+  <si>
+    <t>l22170724@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Johan Abel Camacho Medina</t>
+  </si>
+  <si>
+    <t>l20170618@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Josue Natanael Rojo Payan</t>
+  </si>
+  <si>
+    <t>l24170717@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Victor Hugo Santiso Medin</t>
+  </si>
+  <si>
+    <t>l24170737@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Jesus Cristian Niebla Garcia</t>
+  </si>
+  <si>
+    <t>l24170653@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Angela Imelda Millan Lopez</t>
+  </si>
+  <si>
+    <t>l24170638@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Maria del Rosario Gonzalez Alvarez</t>
+  </si>
+  <si>
+    <t>dato sistemas</t>
+  </si>
+  <si>
+    <t>l21170431@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Miguel Angel Peña Lopez</t>
+  </si>
+  <si>
+    <t>Jaqueline Robles Rios</t>
+  </si>
+  <si>
+    <t>l21170454@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Daniel Alejandro Mendez Diarte</t>
+  </si>
+  <si>
+    <t>l22170722@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Luis Fernando Campos Lopez</t>
+  </si>
+  <si>
+    <t>l22170593@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Adriel Gonzalez Magallanes</t>
+  </si>
+  <si>
+    <t>l24170577@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Juan Axel Torres Ramos</t>
+  </si>
+  <si>
+    <t>l24170750@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Frida Maria Mendoza del Rio</t>
+  </si>
+  <si>
+    <t>l24170627@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Cesar Imanol Elenes Terrazas</t>
+  </si>
+  <si>
+    <t>l22170634@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Kevin Jasiel Samano Machado</t>
+  </si>
+  <si>
+    <t>l22170815@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Javier Enrique Perez Sosa</t>
+  </si>
+  <si>
+    <t>l22170771@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Sebastian Bejarano Ureta</t>
+  </si>
+  <si>
+    <t>l22170574@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Jesus Ricardo Valerio Rodriguez</t>
+  </si>
+  <si>
+    <t>l21170464@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Jesus Antonio Bringas Alvarado</t>
+  </si>
+  <si>
+    <t>l21170264@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CristopherTrapero Orona </t>
+  </si>
+  <si>
+    <t>l21170494@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Juan Eduardo Garcia Noriz</t>
+  </si>
+  <si>
+    <t>l21170335@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Fernando David Loza Moreno</t>
+  </si>
+  <si>
+    <t>l21170381@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Luis Daniel Botello Lopez</t>
+  </si>
+  <si>
+    <t>l23170020@culiacan.tecnm.mx</t>
+  </si>
+  <si>
+    <t>Rosalio Zatarain Cabada</t>
+  </si>
+  <si>
+    <t>Martha Estela Valenzuela Tirado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -319,16 +597,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -345,7 +622,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -661,21 +938,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE89CA4D-4172-7F4C-AFA2-221F0B1D7831}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="2" max="2" width="33.7265625" customWidth="1"/>
+    <col min="3" max="3" width="28.36328125" customWidth="1"/>
+    <col min="5" max="5" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -692,211 +969,211 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>21170348</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>21170273</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>21170305</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>21170398</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>21170421</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>21170259</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>20170855</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>21170502</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" t="s">
-        <v>62</v>
+        <v>68</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>21170291</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>21170434</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>21170432</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>21170235</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>21170302</v>
       </c>
@@ -904,16 +1181,16 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>21170344</v>
       </c>
@@ -921,16 +1198,16 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>21170491</v>
       </c>
@@ -938,101 +1215,101 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>21170361</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>21170517</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>21170263</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>59</v>
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>21170282</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>21170458</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>22170571</v>
       </c>
@@ -1040,118 +1317,115 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>21170409</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>21170229</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>21170387</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>21170000</v>
-      </c>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="B26" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>21170435</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>21170481</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>21170329</v>
       </c>
@@ -1159,50 +1433,50 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>21170512</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>21170338</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>22170720</v>
       </c>
@@ -1210,109 +1484,908 @@
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>21170276</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" t="s">
-        <v>64</v>
+        <v>72</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>21170262</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" t="s">
-        <v>67</v>
+        <v>73</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>21170252</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
-        <v>21170298</v>
+        <v>21170497</v>
       </c>
       <c r="B36" t="s">
         <v>77</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
-        <v>21170236</v>
+        <v>23170214</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D37" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>23170137</v>
+      </c>
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>23170115</v>
+      </c>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>24170747</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>21170550</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>21170433</v>
+      </c>
+      <c r="B43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>23170279</v>
+      </c>
+      <c r="B44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>24270519</v>
+      </c>
+      <c r="B45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>24170488</v>
+      </c>
+      <c r="B46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>24170713</v>
+      </c>
+      <c r="B47" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>23170907</v>
+      </c>
+      <c r="B48" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>24170758</v>
+      </c>
+      <c r="B49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>22170723</v>
+      </c>
+      <c r="B50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>24171226</v>
+      </c>
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>21170694</v>
+      </c>
+      <c r="B52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D52" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>21171174</v>
+      </c>
+      <c r="B53" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>23170044</v>
+      </c>
+      <c r="B54" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>23170037</v>
+      </c>
+      <c r="B55" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D55" t="s">
+        <v>49</v>
+      </c>
+      <c r="E55" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>23170042</v>
+      </c>
+      <c r="B56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56" t="s">
+        <v>49</v>
+      </c>
+      <c r="E56" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>23170054</v>
+      </c>
+      <c r="B57" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D57" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>23170050</v>
+      </c>
+      <c r="B58" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D58" t="s">
+        <v>49</v>
+      </c>
+      <c r="E58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>23170055</v>
+      </c>
+      <c r="B59" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>22170724</v>
+      </c>
+      <c r="B60" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D60" t="s">
+        <v>49</v>
+      </c>
+      <c r="E60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>20170618</v>
+      </c>
+      <c r="B61" t="s">
+        <v>129</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D61" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>24170717</v>
+      </c>
+      <c r="B62" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D62" t="s">
+        <v>49</v>
+      </c>
+      <c r="E62" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>24170737</v>
+      </c>
+      <c r="B63" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E63" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
+        <v>24170653</v>
+      </c>
+      <c r="B64" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D64" t="s">
+        <v>49</v>
+      </c>
+      <c r="E64" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65">
+        <v>24170638</v>
+      </c>
+      <c r="B65" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" t="s">
+        <v>49</v>
+      </c>
+      <c r="E65" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <v>8988</v>
+      </c>
+      <c r="B66" t="s">
+        <v>139</v>
+      </c>
+      <c r="D66" t="s">
+        <v>50</v>
+      </c>
+      <c r="E66" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <v>21170431</v>
+      </c>
+      <c r="B67" t="s">
+        <v>142</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D67" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
+        <v>21170454</v>
+      </c>
+      <c r="B68" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D68" t="s">
+        <v>49</v>
+      </c>
+      <c r="E68" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69">
+        <v>22170722</v>
+      </c>
+      <c r="B69" t="s">
+        <v>145</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D69" t="s">
+        <v>49</v>
+      </c>
+      <c r="E69" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
+        <v>22170593</v>
+      </c>
+      <c r="B70" t="s">
+        <v>147</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D70" t="s">
+        <v>49</v>
+      </c>
+      <c r="E70" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71">
+        <v>24170577</v>
+      </c>
+      <c r="B71" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D71" t="s">
+        <v>49</v>
+      </c>
+      <c r="E71" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72">
+        <v>24170750</v>
+      </c>
+      <c r="B72" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D72" t="s">
+        <v>49</v>
+      </c>
+      <c r="E72" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73">
+        <v>24170627</v>
+      </c>
+      <c r="B73" t="s">
+        <v>153</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D73" t="s">
+        <v>49</v>
+      </c>
+      <c r="E73" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <v>22170634</v>
+      </c>
+      <c r="B74" t="s">
+        <v>155</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D74" t="s">
+        <v>49</v>
+      </c>
+      <c r="E74" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <v>22170815</v>
+      </c>
+      <c r="B75" t="s">
+        <v>157</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D75" t="s">
+        <v>49</v>
+      </c>
+      <c r="E75" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <v>22170771</v>
+      </c>
+      <c r="B76" t="s">
+        <v>159</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D76" t="s">
+        <v>49</v>
+      </c>
+      <c r="E76" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <v>22170574</v>
+      </c>
+      <c r="B77" t="s">
+        <v>161</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D77" t="s">
+        <v>49</v>
+      </c>
+      <c r="E77" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78">
+        <v>21170464</v>
+      </c>
+      <c r="B78" t="s">
+        <v>163</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D78" t="s">
+        <v>49</v>
+      </c>
+      <c r="E78" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79">
+        <v>21170264</v>
+      </c>
+      <c r="B79" t="s">
+        <v>165</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D79" t="s">
+        <v>49</v>
+      </c>
+      <c r="E79" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <v>21170494</v>
+      </c>
+      <c r="B80" t="s">
+        <v>167</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D80" t="s">
+        <v>49</v>
+      </c>
+      <c r="E80" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81">
+        <v>21170335</v>
+      </c>
+      <c r="B81" t="s">
+        <v>169</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D81" t="s">
+        <v>49</v>
+      </c>
+      <c r="E81" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82">
+        <v>21170381</v>
+      </c>
+      <c r="B82" t="s">
+        <v>171</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D82" t="s">
+        <v>49</v>
+      </c>
+      <c r="E82" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83">
+        <v>23170020</v>
+      </c>
+      <c r="B83" t="s">
+        <v>173</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D83" t="s">
+        <v>49</v>
+      </c>
+      <c r="E83" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="2">
+        <v>602</v>
+      </c>
+      <c r="B84" t="s">
+        <v>175</v>
+      </c>
+      <c r="D84" t="s">
+        <v>50</v>
+      </c>
+      <c r="E84" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85">
+        <v>1389</v>
+      </c>
+      <c r="B85" t="s">
+        <v>176</v>
+      </c>
+      <c r="D85" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
     <sortCondition ref="B2:B32"/>
   </sortState>
-  <hyperlinks>
-    <hyperlink ref="C36" r:id="rId1" xr:uid="{EB7733CE-63BF-7346-9EAA-8EB39C20C339}"/>
-    <hyperlink ref="C37" r:id="rId2" xr:uid="{B7755757-3556-2547-81AE-75E70A9AB35A}"/>
-    <hyperlink ref="C35" r:id="rId3" xr:uid="{22672B69-C9F0-BB4C-AC6A-0D2AADC7ADAF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>